<commit_message>
Reparation du body impossible, export en step, fusion de l'objet, puis intégration
</commit_message>
<xml_diff>
--- a/rock_stats.xlsx
+++ b/rock_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\OneDrive\Bureau\INeedToFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFEE98A-8C69-4D20-BACB-480CCEFF95C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1CED7E-E02C-4B17-A402-A8D155E119E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <r>
       <t xml:space="preserve"> g </t>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Fan Total :</t>
+  </si>
+  <si>
+    <t>ESTIMATED PRINTER :</t>
+  </si>
+  <si>
+    <t>108g</t>
   </si>
 </sst>
 </file>
@@ -729,7 +735,7 @@
   <dimension ref="B1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,6 +837,12 @@
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>38</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>

</xml_diff>

<commit_message>
update all parts non testé
</commit_message>
<xml_diff>
--- a/rock_stats.xlsx
+++ b/rock_stats.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\OneDrive\Bureau\INeedToFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515DBE56-CB9C-466F-BD31-A97ECA3F3E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96353BE2-EE9B-4D4B-BA37-2E2F9E1CCE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25305" yWindow="735" windowWidth="21900" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <r>
       <t xml:space="preserve"> g </t>
@@ -238,6 +228,45 @@
   </si>
   <si>
     <t>108g</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Central part</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>bloc_arriere_avec_ailerons</t>
+  </si>
+  <si>
+    <t>motor_casing</t>
+  </si>
+  <si>
+    <t>Anus</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Head_to_body</t>
+  </si>
+  <si>
+    <t>Realité (</t>
+  </si>
+  <si>
+    <t>Poids par piece, estimation / réalité (grammes)</t>
+  </si>
+  <si>
+    <t>Estimation (Cura)</t>
+  </si>
+  <si>
+    <t>Parachute?</t>
+  </si>
+  <si>
+    <t>Moteur?</t>
   </si>
 </sst>
 </file>
@@ -420,7 +449,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1"/>
@@ -439,15 +468,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calcul" xfId="3" builtinId="22"/>
@@ -467,6 +497,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C736AE6-CD78-4DAB-B738-3B7204B65C4D}" name="Tableau1" displayName="Tableau1" ref="B13:D23" totalsRowShown="0">
+  <autoFilter ref="B13:D23" xr:uid="{6C736AE6-CD78-4DAB-B738-3B7204B65C4D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E0CC2539-9CEC-4717-B861-FCF2E19BE23B}" name="Part"/>
+    <tableColumn id="2" xr3:uid="{C44A4296-7E78-4613-BFB3-4ECE38703D2A}" name="Estimation (Cura)"/>
+    <tableColumn id="3" xr3:uid="{0B1DDF5C-2846-4F05-BEC6-C99F51B77C38}" name="Realité ("/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,14 +774,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T17"/>
+  <dimension ref="B1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="8" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="23.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" customWidth="1"/>
     <col min="18" max="18" width="21.28515625" customWidth="1"/>
@@ -753,15 +797,15 @@
       </c>
     </row>
     <row r="2" spans="2:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="M2" s="8" t="s">
         <v>3</v>
       </c>
@@ -773,7 +817,7 @@
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
@@ -795,7 +839,7 @@
       <c r="S3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="10"/>
+      <c r="T3" s="9"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -818,8 +862,8 @@
         <v>9</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
@@ -844,8 +888,8 @@
         <v>38</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -867,8 +911,8 @@
         <v>11</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -888,8 +932,8 @@
       </c>
       <c r="O7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -905,8 +949,8 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -935,8 +979,8 @@
         <v>20.25</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -953,8 +997,8 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
     </row>
     <row r="11" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M11" s="1" t="s">
@@ -968,10 +1012,19 @@
         <v>16</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
     </row>
     <row r="12" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
       <c r="M12" s="1" t="s">
         <v>7</v>
       </c>
@@ -990,18 +1043,36 @@
         <v>29</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
     </row>
     <row r="13" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>57</v>
+      </c>
       <c r="M14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1012,10 +1083,19 @@
         <v>22</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
       <c r="M15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1034,29 +1114,89 @@
         <v>29</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-    </row>
-    <row r="17" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f>SUM(C14:C22)</f>
+        <v>216</v>
+      </c>
+      <c r="D25">
+        <f>SUM(D14:D22)</f>
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="M2:T2"/>
     <mergeCell ref="S3:T17"/>
     <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update infos on rocket with current weight
</commit_message>
<xml_diff>
--- a/rock_stats.xlsx
+++ b/rock_stats.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\OneDrive\Bureau\INeedToFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96353BE2-EE9B-4D4B-BA37-2E2F9E1CCE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE67B73-5269-46A3-8BC5-41CBEF14AC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rocket_stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Rocket infos to discuss" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <r>
       <t xml:space="preserve"> g </t>
@@ -251,9 +263,6 @@
     <t>Head</t>
   </si>
   <si>
-    <t>Head_to_body</t>
-  </si>
-  <si>
     <t>Realité (</t>
   </si>
   <si>
@@ -267,13 +276,34 @@
   </si>
   <si>
     <t>Moteur?</t>
+  </si>
+  <si>
+    <t>Head_to_body (80% print)</t>
+  </si>
+  <si>
+    <t>without motur</t>
+  </si>
+  <si>
+    <t>with moteur</t>
+  </si>
+  <si>
+    <t>Thicness of rocket is 2mm, i think we can lower</t>
+  </si>
+  <si>
+    <t>did it survive ground test lunch?</t>
+  </si>
+  <si>
+    <t>3D print is imperfect for "long","high" tube without support, need to reprint</t>
+  </si>
+  <si>
+    <t>does bottom to top is strong enough ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +373,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -449,7 +487,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1"/>
@@ -468,16 +506,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calcul" xfId="3" builtinId="22"/>
@@ -774,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T25"/>
+  <dimension ref="B1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,15 +840,15 @@
       </c>
     </row>
     <row r="2" spans="2:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
       <c r="M2" s="8" t="s">
         <v>3</v>
       </c>
@@ -862,8 +905,8 @@
         <v>9</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
     </row>
     <row r="5" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
@@ -876,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="7">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>14</v>
@@ -888,8 +931,8 @@
         <v>38</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -911,8 +954,8 @@
         <v>11</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -932,8 +975,8 @@
       </c>
       <c r="O7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -949,8 +992,8 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -979,8 +1022,8 @@
         <v>20.25</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -997,8 +1040,8 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="11" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M11" s="1" t="s">
@@ -1006,62 +1049,58 @@
       </c>
       <c r="N11" s="5">
         <f>((N4*N5*2)/(N6*N7*Q9))</f>
-        <v>0.31637188208616779</v>
+        <v>0.25309750566893424</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
     </row>
     <row r="12" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="B12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="M12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N12" s="5">
         <f>( (  (4*N11)/PI()  )^(1/2) )</f>
-        <v>0.63467880941023924</v>
+        <v>0.56767398468797126</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="P12">
         <f>(N12/0.0254)</f>
-        <v>24.987354701190522</v>
+        <v>22.349369475904382</v>
       </c>
       <c r="Q12" t="s">
         <v>29</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1083,8 +1122,8 @@
         <v>22</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1101,21 +1140,21 @@
       </c>
       <c r="N15" s="1">
         <f>(N12*(1+(N14/100)))</f>
-        <v>0.6981466903512632</v>
+        <v>0.62444138315676845</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="P15">
         <f>(N15/0.0254)</f>
-        <v>27.486090171309577</v>
+        <v>24.584306423494823</v>
       </c>
       <c r="Q15" t="s">
         <v>29</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1123,13 +1162,16 @@
       </c>
       <c r="C16">
         <v>47</v>
+      </c>
+      <c r="D16">
+        <v>38</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1138,9 +1180,12 @@
       <c r="C17">
         <v>10</v>
       </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1157,33 +1202,58 @@
       <c r="C19">
         <v>24</v>
       </c>
+      <c r="D19">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <f>SUM(D19:D20)</f>
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>25</v>
       </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
       <c r="C25">
         <f>SUM(C14:C22)</f>
         <v>216</v>
       </c>
       <c r="D25">
         <f>SUM(D14:D22)</f>
-        <v>84</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <f>SUM(D23,D25)</f>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1199,4 +1269,43 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FB27BC-9873-47D2-8DE9-ACE05E4A1B4C}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upate, correct mortor size wit anus and weight
</commit_message>
<xml_diff>
--- a/rock_stats.xlsx
+++ b/rock_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\OneDrive\Bureau\INeedToFly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE67B73-5269-46A3-8BC5-41CBEF14AC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CA65C-BCAF-4806-B879-D5B78E901241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26640" yWindow="-2850" windowWidth="26760" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rocket_stats" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <r>
       <t xml:space="preserve"> g </t>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>does bottom to top is strong enough ?</t>
+  </si>
+  <si>
+    <t>Motor D size is :</t>
+  </si>
+  <si>
+    <t>longueur</t>
+  </si>
+  <si>
+    <t>68,3mm</t>
+  </si>
+  <si>
+    <t>largeur 17,8</t>
   </si>
 </sst>
 </file>
@@ -500,6 +512,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,12 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -819,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,25 +852,25 @@
       </c>
     </row>
     <row r="2" spans="2:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="M2" s="8" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="M2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="2:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -879,10 +891,10 @@
       <c r="R3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="9"/>
+      <c r="T3" s="11"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -905,8 +917,8 @@
         <v>9</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
@@ -931,8 +943,8 @@
         <v>38</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -954,8 +966,8 @@
         <v>11</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -975,8 +987,8 @@
       </c>
       <c r="O7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -992,8 +1004,8 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -1022,8 +1034,8 @@
         <v>20.25</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -1040,8 +1052,8 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
     </row>
     <row r="11" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M11" s="1" t="s">
@@ -1055,15 +1067,15 @@
         <v>16</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
     </row>
     <row r="12" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="M12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1082,8 +1094,8 @@
         <v>29</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
     </row>
     <row r="13" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1099,8 +1111,8 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1122,8 +1134,8 @@
         <v>22</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1153,8 +1165,8 @@
         <v>29</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1170,8 +1182,8 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1184,8 +1196,8 @@
         <v>6</v>
       </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1246,6 +1258,17 @@
         <f>SUM(D14:D22)</f>
         <v>200</v>
       </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1254,6 +1277,9 @@
       <c r="D27">
         <f>SUM(D23,D25)</f>
         <v>227</v>
+      </c>
+      <c r="H27" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1275,31 +1301,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FB27BC-9873-47D2-8DE9-ACE05E4A1B4C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>